<commit_message>
Ajout des commentaires et ajout des quantités si produit deja present à la page product
</commit_message>
<xml_diff>
--- a/Modèle-plan-tests-acceptation.xlsx
+++ b/Modèle-plan-tests-acceptation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpira\Desktop\Formation\P5_pirat_geoffrey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D06FAA57-1B66-45C8-B573-40F9B817DFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4C3F5B-05E2-4272-8F99-7485A915A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -43,10 +43,28 @@
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>OK / Description erreur</t>
-  </si>
-  <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>Affichage le canapé selectionné</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Une page panier qui récapitule la sélection des produits, sa quantité total ainsi que son prix total.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page produit du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Affiche le récapitulatif de la commande</t>
+  </si>
+  <si>
+    <t>Une page produit qui une fois le canapé sélectionné de la page d'accueil, redirige sur celle-ci et montre ses informations détaillées, le choix de sa couleur, sa quantité.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page panier du site web dans un navigateur</t>
   </si>
 </sst>
 </file>
@@ -339,9 +357,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -357,18 +372,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -388,6 +391,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -610,8 +628,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -638,172 +656,188 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="77.599999999999994" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" ht="77.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="87.45" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A10" s="14"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A14" s="14"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A16" s="14"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A18" s="14"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A20" s="14"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A21" s="14"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" ht="17.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A9" s="9"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A10" s="9"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A13" s="9"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A14" s="9"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A15" s="9"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A16" s="9"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A17" s="9"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A18" s="9"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A19" s="9"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A20" s="9"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A21" s="9"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modele plan test completé
</commit_message>
<xml_diff>
--- a/Modèle-plan-tests-acceptation.xlsx
+++ b/Modèle-plan-tests-acceptation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpira\Desktop\Formation\P5_pirat_geoffrey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4C3F5B-05E2-4272-8F99-7485A915A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB38C14-1AA8-414A-BA2E-135F4A0C105A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -37,34 +37,94 @@
     <t>Une page d’accueil montrant (de manière dynamique) tous les articles disponibles à la vente.</t>
   </si>
   <si>
-    <t>Ouvrir sur la page d'accueil du site web dans un navigateur</t>
-  </si>
-  <si>
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
-    <t>Affichage le canapé selectionné</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>Une page panier qui récapitule la sélection des produits, sa quantité total ainsi que son prix total.</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page produit du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t>Affiche le récapitulatif de la commande</t>
-  </si>
-  <si>
-    <t>Une page produit qui une fois le canapé sélectionné de la page d'accueil, redirige sur celle-ci et montre ses informations détaillées, le choix de sa couleur, sa quantité.</t>
-  </si>
-  <si>
     <t>Ouvrir sur la page panier du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t>Depuis la page produit, bouton qui permet d'ajouter au panier l'article définie</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page produit du site web dans un navigateur.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page d'accueil du site web dans un navigateur.</t>
+  </si>
+  <si>
+    <t>Si la quantité est supérieur à 0, enregistre les informations de l'article, ses informations, sa couleur et sa quantité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enregistre les informations de l'article, sa couleur et quantité dans le localstorage </t>
+  </si>
+  <si>
+    <t>Depuis la page panier, possibilité de modifier la quantité de l'article, ou bien de le supprimer.</t>
+  </si>
+  <si>
+    <t>Affiche la quantité et le boutton "supprimer" de l'article.</t>
+  </si>
+  <si>
+    <t>Redirige vers la page confirmation pour afficher le numéro de la commande.</t>
+  </si>
+  <si>
+    <t>Vérifie et envoie les données du panier et du formulaire au serveur.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page confirmation du site web dans un navigateur.</t>
+  </si>
+  <si>
+    <t>Affiche un message indiquant que la commande est valide avec le numéro de commande.</t>
+  </si>
+  <si>
+    <t>Depuis la page produit, affiche un menu déroulant qui contient les différentes couleurs de l'article  récupérées depuis l'API du serveur.</t>
+  </si>
+  <si>
+    <t>Affiche la couleur sélectionnée du menu déroulant.</t>
+  </si>
+  <si>
+    <t>Affiche le chiffre rentré par l'utilisateur et lui permet de le modifier.</t>
+  </si>
+  <si>
+    <t>Affichage le canapé selectionné et ses informations, un menu déroulant pour le choix de la couleur, un input pour définir la quantité, ainsi qu'un boutton "Ajouter au panier".</t>
+  </si>
+  <si>
+    <t>Modification de la quantité ou suppression de l'article puis sauvegarde la quantité dans le localstorage.</t>
+  </si>
+  <si>
+    <t>Affiche un menu déroulant. Celui-ci contient les différentes couleurs possible.</t>
+  </si>
+  <si>
+    <t>Affiche un input. Il permettra la définition de la quantité par le chiffre rentré par l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Depuis la page produit, possibilité de définir la quantité de l'article voulue en entrant un chiffre dans un input et/ou d'augmenter de diminuer sa quantité par un clic sur icone fléché.</t>
+  </si>
+  <si>
+    <t>Une page produit montrant (de manière dynamique)  l'article sélectionné depuis la page d'accueil, les informations détaillées de celui-ci, le choix de sa couleur et de sa quantité, ainsi qu'un boutton "Ajouter au panier".</t>
+  </si>
+  <si>
+    <t>Une page panier montrant (de manière dynamique) le récapitulatif des articles ajouté au panier depuis la page produit, la possibilité de changer la quantité ou de supprimer un article en particulier. Un récapitulatif de la quantité et du prix total de tous les articles sélectionnés. Possédant un formulaire ainsi qu'un boutton "Commander !"</t>
+  </si>
+  <si>
+    <t>Affiche le récapitulatif de la commande, le choix de modifier la quantité de l'article et la possiblilité de le supprimer, un formulaire, le bouton "Commander !"</t>
+  </si>
+  <si>
+    <t>Affichage du formulaire, dont l'utilisateur peut rentrer des informations dans les inputs.</t>
+  </si>
+  <si>
+    <t>Depuis la page panier, boutton "Commander !" qui permet d'envoyer les informations récoltées du panier et du formulaire au serveur si celles-ci sont valide.</t>
+  </si>
+  <si>
+    <t>Affiche un formulaire, si données valides, bordure verte autour de l'input et sinon, bordure rouge avec message d'erreur.</t>
+  </si>
+  <si>
+    <t>Depuis la page panier, formulaire permettant de récolter les informations entrées par l'utilisateur de son prénom, nom, adresse, ville et email et de vérifier si celles-ci sont valides. Si valides, bordure verte autour de l'input pour indiquer que données OK, sinon bordure rouge et message d'erreur.</t>
+  </si>
+  <si>
+    <t>Une page confirmation montrant (de manière dynamique) un message de validation de la commande avec son numéro de commande généré par le serveur.</t>
   </si>
 </sst>
 </file>
@@ -343,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -356,9 +416,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -626,10 +683,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -657,187 +714,258 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="77.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="109.3" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="87.45" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
+      <c r="D3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="65.599999999999994" x14ac:dyDescent="0.7">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="87.45" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="65.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="153" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="65.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="C8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="131.15" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
         <v>8</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="B9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="87.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="20">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="B10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="87.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
         <v>10</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A12" s="9"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A13" s="9"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A14" s="9"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A15" s="9"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A16" s="9"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A17" s="9"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A18" s="9"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A19" s="9"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A20" s="9"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A21" s="9"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" ht="21.9" x14ac:dyDescent="0.7">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>